<commit_message>
grand prize functional dependencies : matrix preparation
</commit_message>
<xml_diff>
--- a/FOAD_MERISE/grand_prix.xlsx
+++ b/FOAD_MERISE/grand_prix.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23120"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4CE2EFF9-F30C-4EE3-837C-6B53D4505CDC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E3B405CA-60AA-4CAF-9F77-AC64228254AF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="52">
   <si>
     <t>dictionnaire des données</t>
   </si>
@@ -105,7 +105,7 @@
     <t>entier</t>
   </si>
   <si>
-    <t>athleticsMeet</t>
+    <t>athleticMeet</t>
   </si>
   <si>
     <t>am_date</t>
@@ -136,6 +136,51 @@
   </si>
   <si>
     <t>facultatif</t>
+  </si>
+  <si>
+    <t>dépendances fonctionnelles</t>
+  </si>
+  <si>
+    <t>GRANDPRIZE</t>
+  </si>
+  <si>
+    <t>SPORTFEDERATION</t>
+  </si>
+  <si>
+    <t>ATHLETE</t>
+  </si>
+  <si>
+    <t>ATLEHTICMEET</t>
+  </si>
+  <si>
+    <t>TEST</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>firstname</t>
+  </si>
+  <si>
+    <t>lastname</t>
+  </si>
+  <si>
+    <t>specialty</t>
+  </si>
+  <si>
+    <t>score</t>
+  </si>
+  <si>
+    <t>location</t>
+  </si>
+  <si>
+    <t>discipline</t>
+  </si>
+  <si>
+    <t>max_participant</t>
   </si>
 </sst>
 </file>
@@ -167,7 +212,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -204,8 +249,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDDEBF7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE7E6E6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -228,11 +285,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -242,6 +312,23 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -556,9 +643,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:L37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -566,8 +655,9 @@
     <col min="2" max="2" width="19.28515625" customWidth="1"/>
     <col min="3" max="3" width="29.28515625" customWidth="1"/>
     <col min="4" max="4" width="24.140625" customWidth="1"/>
-    <col min="5" max="5" width="20.7109375" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" customWidth="1"/>
     <col min="7" max="7" width="14" customWidth="1"/>
+    <col min="12" max="12" width="16.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15.75">
@@ -748,7 +838,7 @@
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:12">
       <c r="A17" s="7" t="s">
         <v>31</v>
       </c>
@@ -765,7 +855,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:12">
       <c r="A18" s="2"/>
       <c r="B18" s="7" t="s">
         <v>34</v>
@@ -780,7 +870,293 @@
         <v>36</v>
       </c>
     </row>
+    <row r="20" spans="1:12">
+      <c r="A20" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12">
+      <c r="C22" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="E22" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="F22" s="10"/>
+      <c r="G22" s="10"/>
+      <c r="H22" s="10"/>
+      <c r="I22" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="J22" s="11"/>
+      <c r="K22" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="L22" s="12"/>
+    </row>
+    <row r="23" spans="1:12">
+      <c r="C23" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="F23" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="G23" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="H23" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="I23" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="J23" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="K23" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="L23" s="13" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12">
+      <c r="C24" s="9"/>
+      <c r="D24" s="4"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5"/>
+      <c r="G24" s="5"/>
+      <c r="H24" s="5"/>
+      <c r="I24" s="6"/>
+      <c r="J24" s="6"/>
+      <c r="K24" s="13"/>
+      <c r="L24" s="13"/>
+    </row>
+    <row r="25" spans="1:12">
+      <c r="A25" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B25" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="C25" s="14"/>
+      <c r="D25" s="4"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="5"/>
+      <c r="G25" s="5"/>
+      <c r="H25" s="5"/>
+      <c r="I25" s="6"/>
+      <c r="J25" s="6"/>
+      <c r="K25" s="13"/>
+      <c r="L25" s="13"/>
+    </row>
+    <row r="26" spans="1:12">
+      <c r="A26" s="2"/>
+      <c r="B26" s="2"/>
+      <c r="C26" s="15"/>
+      <c r="D26" s="4"/>
+      <c r="E26" s="5"/>
+      <c r="F26" s="5"/>
+      <c r="G26" s="5"/>
+      <c r="H26" s="5"/>
+      <c r="I26" s="6"/>
+      <c r="J26" s="6"/>
+      <c r="K26" s="13"/>
+      <c r="L26" s="13"/>
+    </row>
+    <row r="27" spans="1:12">
+      <c r="A27" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C27" s="16"/>
+      <c r="D27" s="4"/>
+      <c r="E27" s="5"/>
+      <c r="F27" s="5"/>
+      <c r="G27" s="5"/>
+      <c r="H27" s="5"/>
+      <c r="I27" s="6"/>
+      <c r="J27" s="6"/>
+      <c r="K27" s="13"/>
+      <c r="L27" s="13"/>
+    </row>
+    <row r="28" spans="1:12">
+      <c r="A28" s="2"/>
+      <c r="B28" s="2"/>
+      <c r="C28" s="15"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="5"/>
+      <c r="F28" s="5"/>
+      <c r="G28" s="5"/>
+      <c r="H28" s="5"/>
+      <c r="I28" s="6"/>
+      <c r="J28" s="6"/>
+      <c r="K28" s="13"/>
+      <c r="L28" s="13"/>
+    </row>
+    <row r="29" spans="1:12">
+      <c r="A29" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C29" s="17"/>
+      <c r="D29" s="5"/>
+      <c r="E29" s="5"/>
+      <c r="F29" s="5"/>
+      <c r="G29" s="5"/>
+      <c r="H29" s="5"/>
+      <c r="I29" s="6"/>
+      <c r="J29" s="6"/>
+      <c r="K29" s="13"/>
+      <c r="L29" s="13"/>
+    </row>
+    <row r="30" spans="1:12">
+      <c r="A30" s="2"/>
+      <c r="B30" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C30" s="17"/>
+      <c r="D30" s="5"/>
+      <c r="E30" s="5"/>
+      <c r="F30" s="5"/>
+      <c r="G30" s="5"/>
+      <c r="H30" s="5"/>
+      <c r="I30" s="6"/>
+      <c r="J30" s="6"/>
+      <c r="K30" s="13"/>
+      <c r="L30" s="13"/>
+    </row>
+    <row r="31" spans="1:12">
+      <c r="A31" s="2"/>
+      <c r="B31" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C31" s="17"/>
+      <c r="D31" s="5"/>
+      <c r="E31" s="5"/>
+      <c r="F31" s="5"/>
+      <c r="G31" s="5"/>
+      <c r="H31" s="5"/>
+      <c r="I31" s="6"/>
+      <c r="J31" s="6"/>
+      <c r="K31" s="13"/>
+      <c r="L31" s="13"/>
+    </row>
+    <row r="32" spans="1:12">
+      <c r="A32" s="2"/>
+      <c r="B32" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C32" s="17"/>
+      <c r="D32" s="5"/>
+      <c r="E32" s="5"/>
+      <c r="F32" s="5"/>
+      <c r="G32" s="5"/>
+      <c r="H32" s="5"/>
+      <c r="I32" s="6"/>
+      <c r="J32" s="6"/>
+      <c r="K32" s="13"/>
+      <c r="L32" s="13"/>
+    </row>
+    <row r="33" spans="1:12">
+      <c r="A33" s="2"/>
+      <c r="B33" s="2"/>
+      <c r="C33" s="15"/>
+      <c r="D33" s="2"/>
+      <c r="E33" s="2"/>
+      <c r="F33" s="2"/>
+      <c r="G33" s="2"/>
+      <c r="H33" s="2"/>
+      <c r="I33" s="6"/>
+      <c r="J33" s="6"/>
+      <c r="K33" s="13"/>
+      <c r="L33" s="13"/>
+    </row>
+    <row r="34" spans="1:12">
+      <c r="A34" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="B34" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C34" s="18"/>
+      <c r="D34" s="6"/>
+      <c r="E34" s="6"/>
+      <c r="F34" s="6"/>
+      <c r="G34" s="6"/>
+      <c r="H34" s="6"/>
+      <c r="I34" s="6"/>
+      <c r="J34" s="6"/>
+      <c r="K34" s="13"/>
+      <c r="L34" s="13"/>
+    </row>
+    <row r="35" spans="1:12">
+      <c r="A35" s="2"/>
+      <c r="B35" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C35" s="18"/>
+      <c r="D35" s="6"/>
+      <c r="E35" s="6"/>
+      <c r="F35" s="6"/>
+      <c r="G35" s="6"/>
+      <c r="H35" s="6"/>
+      <c r="I35" s="6"/>
+      <c r="J35" s="6"/>
+      <c r="K35" s="13"/>
+      <c r="L35" s="13"/>
+    </row>
+    <row r="36" spans="1:12">
+      <c r="A36" s="2"/>
+      <c r="B36" s="2"/>
+      <c r="C36" s="15"/>
+      <c r="D36" s="2"/>
+      <c r="E36" s="2"/>
+      <c r="F36" s="2"/>
+      <c r="G36" s="2"/>
+      <c r="H36" s="2"/>
+      <c r="I36" s="2"/>
+      <c r="J36" s="2"/>
+      <c r="K36" s="13"/>
+      <c r="L36" s="13"/>
+    </row>
+    <row r="37" spans="1:12">
+      <c r="A37" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="B37" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="C37" s="19"/>
+      <c r="D37" s="13"/>
+      <c r="E37" s="13"/>
+      <c r="F37" s="13"/>
+      <c r="G37" s="13"/>
+      <c r="H37" s="13"/>
+      <c r="I37" s="13"/>
+      <c r="J37" s="13"/>
+      <c r="K37" s="13"/>
+      <c r="L37" s="13"/>
+    </row>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="E22:H22"/>
+    <mergeCell ref="I22:J22"/>
+    <mergeCell ref="K22:L22"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
grand prize update dictionnary + functionnal dependencies
</commit_message>
<xml_diff>
--- a/FOAD_MERISE/grand_prix.xlsx
+++ b/FOAD_MERISE/grand_prix.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23120"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E3B405CA-60AA-4CAF-9F77-AC64228254AF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E212E005-9669-400F-A666-3C4C0090ECE9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="56">
   <si>
     <t>dictionnaire des données</t>
   </si>
@@ -87,15 +87,24 @@
     <t>nom de famille de l'athlète</t>
   </si>
   <si>
+    <t>athlete_gender</t>
+  </si>
+  <si>
+    <t>sexe de l'athlète</t>
+  </si>
+  <si>
+    <t>alphabétique(1)</t>
+  </si>
+  <si>
+    <t>obligatoire</t>
+  </si>
+  <si>
     <t>athlete_specialty</t>
   </si>
   <si>
     <t>spécialité de l'athlète</t>
   </si>
   <si>
-    <t>obligatoire</t>
-  </si>
-  <si>
     <t>athlete_score</t>
   </si>
   <si>
@@ -166,6 +175,9 @@
   </si>
   <si>
     <t>lastname</t>
+  </si>
+  <si>
+    <t>gender</t>
   </si>
   <si>
     <t>specialty</t>
@@ -262,7 +274,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -298,11 +310,35 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -313,15 +349,6 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -329,6 +356,24 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -643,10 +688,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L37"/>
+  <dimension ref="A1:M39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -656,8 +701,8 @@
     <col min="3" max="3" width="29.28515625" customWidth="1"/>
     <col min="4" max="4" width="24.140625" customWidth="1"/>
     <col min="5" max="5" width="12.7109375" customWidth="1"/>
-    <col min="7" max="7" width="14" customWidth="1"/>
-    <col min="12" max="12" width="16.5703125" customWidth="1"/>
+    <col min="8" max="8" width="14" customWidth="1"/>
+    <col min="13" max="13" width="16.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15.75">
@@ -771,61 +816,61 @@
         <v>21</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="2"/>
       <c r="B12" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E12" s="5" t="s">
         <v>23</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="E12" s="5" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="2"/>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
+      <c r="B13" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="14" spans="1:5">
-      <c r="A14" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="D14" s="6" t="s">
+      <c r="A14" s="2"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D15" s="6" t="s">
         <v>9</v>
-      </c>
-      <c r="E14" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5">
-      <c r="A15" s="2"/>
-      <c r="B15" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="D15" s="6" t="s">
-        <v>14</v>
       </c>
       <c r="E15" s="6" t="s">
         <v>10</v>
@@ -833,329 +878,388 @@
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="2"/>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-    </row>
-    <row r="17" spans="1:12">
-      <c r="A17" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="B17" s="7" t="s">
+      <c r="B16" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C17" s="7" t="s">
+      <c r="C16" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="D17" s="7" t="s">
+      <c r="D16" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="E17" s="7" t="s">
+      <c r="E16" s="6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:12">
-      <c r="A18" s="2"/>
+    <row r="17" spans="1:13">
+      <c r="A17" s="2"/>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+    </row>
+    <row r="18" spans="1:13">
+      <c r="A18" s="7" t="s">
+        <v>34</v>
+      </c>
       <c r="B18" s="7" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12">
-      <c r="A20" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13">
+      <c r="A19" s="2"/>
+      <c r="B19" s="7" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="22" spans="1:12">
-      <c r="C22" s="9" t="s">
+      <c r="C19" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="D22" s="4" t="s">
+      <c r="D19" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E19" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="E22" s="10" t="s">
+    </row>
+    <row r="21" spans="1:13">
+      <c r="A21" t="s">
         <v>40</v>
       </c>
-      <c r="F22" s="10"/>
-      <c r="G22" s="10"/>
-      <c r="H22" s="10"/>
-      <c r="I22" s="11" t="s">
+    </row>
+    <row r="23" spans="1:13">
+      <c r="C23" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="J22" s="11"/>
-      <c r="K22" s="12" t="s">
+      <c r="D23" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="L22" s="12"/>
-    </row>
-    <row r="23" spans="1:12">
-      <c r="C23" s="9" t="s">
+      <c r="E23" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="D23" s="4" t="s">
+      <c r="F23" s="22"/>
+      <c r="G23" s="22"/>
+      <c r="H23" s="22"/>
+      <c r="I23" s="20"/>
+      <c r="J23" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="E23" s="5" t="s">
+      <c r="K23" s="17"/>
+      <c r="L23" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="F23" s="5" t="s">
+      <c r="M23" s="18"/>
+    </row>
+    <row r="24" spans="1:13">
+      <c r="C24" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="G23" s="5" t="s">
+      <c r="D24" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="H23" s="5" t="s">
+      <c r="E24" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="I23" s="6" t="s">
+      <c r="F24" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="G24" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="H24" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="I24" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="J24" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="J23" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="K23" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="L23" s="13" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12">
-      <c r="C24" s="9"/>
-      <c r="D24" s="4"/>
-      <c r="E24" s="5"/>
-      <c r="F24" s="5"/>
-      <c r="G24" s="5"/>
-      <c r="H24" s="5"/>
-      <c r="I24" s="6"/>
-      <c r="J24" s="6"/>
-      <c r="K24" s="13"/>
-      <c r="L24" s="13"/>
-    </row>
-    <row r="25" spans="1:12">
-      <c r="A25" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="B25" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="C25" s="14"/>
+      <c r="K24" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="L24" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="M24" s="10" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13">
+      <c r="C25" s="9"/>
       <c r="D25" s="4"/>
       <c r="E25" s="5"/>
       <c r="F25" s="5"/>
       <c r="G25" s="5"/>
       <c r="H25" s="5"/>
-      <c r="I25" s="6"/>
+      <c r="I25" s="5"/>
       <c r="J25" s="6"/>
-      <c r="K25" s="13"/>
-      <c r="L25" s="13"/>
-    </row>
-    <row r="26" spans="1:12">
-      <c r="A26" s="2"/>
-      <c r="B26" s="2"/>
-      <c r="C26" s="15"/>
+      <c r="K25" s="6"/>
+      <c r="L25" s="10"/>
+      <c r="M25" s="10"/>
+    </row>
+    <row r="26" spans="1:13">
+      <c r="A26" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B26" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C26" s="11"/>
       <c r="D26" s="4"/>
       <c r="E26" s="5"/>
       <c r="F26" s="5"/>
       <c r="G26" s="5"/>
       <c r="H26" s="5"/>
-      <c r="I26" s="6"/>
+      <c r="I26" s="5"/>
       <c r="J26" s="6"/>
-      <c r="K26" s="13"/>
-      <c r="L26" s="13"/>
-    </row>
-    <row r="27" spans="1:12">
-      <c r="A27" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="B27" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="C27" s="16"/>
+      <c r="K26" s="6"/>
+      <c r="L26" s="10"/>
+      <c r="M26" s="10"/>
+    </row>
+    <row r="27" spans="1:13">
+      <c r="A27" s="2"/>
+      <c r="B27" s="2"/>
+      <c r="C27" s="12"/>
       <c r="D27" s="4"/>
       <c r="E27" s="5"/>
       <c r="F27" s="5"/>
       <c r="G27" s="5"/>
       <c r="H27" s="5"/>
-      <c r="I27" s="6"/>
+      <c r="I27" s="5"/>
       <c r="J27" s="6"/>
-      <c r="K27" s="13"/>
-      <c r="L27" s="13"/>
-    </row>
-    <row r="28" spans="1:12">
-      <c r="A28" s="2"/>
-      <c r="B28" s="2"/>
-      <c r="C28" s="15"/>
-      <c r="D28" s="2"/>
+      <c r="K27" s="6"/>
+      <c r="L27" s="10"/>
+      <c r="M27" s="10"/>
+    </row>
+    <row r="28" spans="1:13">
+      <c r="A28" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C28" s="13"/>
+      <c r="D28" s="4"/>
       <c r="E28" s="5"/>
       <c r="F28" s="5"/>
       <c r="G28" s="5"/>
       <c r="H28" s="5"/>
-      <c r="I28" s="6"/>
+      <c r="I28" s="5"/>
       <c r="J28" s="6"/>
-      <c r="K28" s="13"/>
-      <c r="L28" s="13"/>
-    </row>
-    <row r="29" spans="1:12">
-      <c r="A29" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="B29" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="C29" s="17"/>
-      <c r="D29" s="5"/>
+      <c r="K28" s="6"/>
+      <c r="L28" s="10"/>
+      <c r="M28" s="10"/>
+    </row>
+    <row r="29" spans="1:13">
+      <c r="A29" s="2"/>
+      <c r="B29" s="2"/>
+      <c r="C29" s="12"/>
+      <c r="D29" s="2"/>
       <c r="E29" s="5"/>
       <c r="F29" s="5"/>
       <c r="G29" s="5"/>
       <c r="H29" s="5"/>
-      <c r="I29" s="6"/>
+      <c r="I29" s="5"/>
       <c r="J29" s="6"/>
-      <c r="K29" s="13"/>
-      <c r="L29" s="13"/>
-    </row>
-    <row r="30" spans="1:12">
-      <c r="A30" s="2"/>
+      <c r="K29" s="6"/>
+      <c r="L29" s="10"/>
+      <c r="M29" s="10"/>
+    </row>
+    <row r="30" spans="1:13">
+      <c r="A30" s="5" t="s">
+        <v>43</v>
+      </c>
       <c r="B30" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="C30" s="17"/>
+        <v>48</v>
+      </c>
+      <c r="C30" s="14"/>
       <c r="D30" s="5"/>
       <c r="E30" s="5"/>
       <c r="F30" s="5"/>
       <c r="G30" s="5"/>
       <c r="H30" s="5"/>
-      <c r="I30" s="6"/>
+      <c r="I30" s="5"/>
       <c r="J30" s="6"/>
-      <c r="K30" s="13"/>
-      <c r="L30" s="13"/>
-    </row>
-    <row r="31" spans="1:12">
+      <c r="K30" s="6"/>
+      <c r="L30" s="10"/>
+      <c r="M30" s="10"/>
+    </row>
+    <row r="31" spans="1:13">
       <c r="A31" s="2"/>
       <c r="B31" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="C31" s="17"/>
+        <v>49</v>
+      </c>
+      <c r="C31" s="14"/>
       <c r="D31" s="5"/>
       <c r="E31" s="5"/>
       <c r="F31" s="5"/>
       <c r="G31" s="5"/>
       <c r="H31" s="5"/>
-      <c r="I31" s="6"/>
+      <c r="I31" s="5"/>
       <c r="J31" s="6"/>
-      <c r="K31" s="13"/>
-      <c r="L31" s="13"/>
-    </row>
-    <row r="32" spans="1:12">
+      <c r="K31" s="6"/>
+      <c r="L31" s="10"/>
+      <c r="M31" s="10"/>
+    </row>
+    <row r="32" spans="1:13">
       <c r="A32" s="2"/>
       <c r="B32" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="C32" s="17"/>
+        <v>50</v>
+      </c>
+      <c r="C32" s="14"/>
       <c r="D32" s="5"/>
-      <c r="E32" s="5"/>
-      <c r="F32" s="5"/>
-      <c r="G32" s="5"/>
+      <c r="E32" s="19">
+        <v>1</v>
+      </c>
+      <c r="F32" s="20"/>
+      <c r="G32" s="14"/>
       <c r="H32" s="5"/>
-      <c r="I32" s="6"/>
+      <c r="I32" s="5"/>
       <c r="J32" s="6"/>
-      <c r="K32" s="13"/>
-      <c r="L32" s="13"/>
-    </row>
-    <row r="33" spans="1:12">
+      <c r="K32" s="6"/>
+      <c r="L32" s="10"/>
+      <c r="M32" s="10"/>
+    </row>
+    <row r="33" spans="1:13">
       <c r="A33" s="2"/>
-      <c r="B33" s="2"/>
-      <c r="C33" s="15"/>
-      <c r="D33" s="2"/>
-      <c r="E33" s="2"/>
-      <c r="F33" s="2"/>
-      <c r="G33" s="2"/>
-      <c r="H33" s="2"/>
-      <c r="I33" s="6"/>
+      <c r="B33" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C33" s="14"/>
+      <c r="D33" s="5"/>
+      <c r="E33" s="19">
+        <v>1</v>
+      </c>
+      <c r="F33" s="20"/>
+      <c r="G33" s="21"/>
+      <c r="H33" s="5"/>
+      <c r="I33" s="5"/>
       <c r="J33" s="6"/>
-      <c r="K33" s="13"/>
-      <c r="L33" s="13"/>
-    </row>
-    <row r="34" spans="1:12">
-      <c r="A34" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="B34" s="6" t="s">
+      <c r="K33" s="6"/>
+      <c r="L33" s="10"/>
+      <c r="M33" s="10"/>
+    </row>
+    <row r="34" spans="1:13">
+      <c r="A34" s="2"/>
+      <c r="B34" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C34" s="14"/>
+      <c r="D34" s="5"/>
+      <c r="E34" s="19">
+        <v>1</v>
+      </c>
+      <c r="F34" s="20"/>
+      <c r="G34" s="21"/>
+      <c r="H34" s="5"/>
+      <c r="I34" s="5"/>
+      <c r="J34" s="6"/>
+      <c r="K34" s="6"/>
+      <c r="L34" s="10"/>
+      <c r="M34" s="10"/>
+    </row>
+    <row r="35" spans="1:13">
+      <c r="A35" s="2"/>
+      <c r="B35" s="2"/>
+      <c r="C35" s="12"/>
+      <c r="D35" s="2"/>
+      <c r="E35" s="2"/>
+      <c r="F35" s="2"/>
+      <c r="G35" s="2"/>
+      <c r="H35" s="2"/>
+      <c r="I35" s="2"/>
+      <c r="J35" s="6"/>
+      <c r="K35" s="6"/>
+      <c r="L35" s="10"/>
+      <c r="M35" s="10"/>
+    </row>
+    <row r="36" spans="1:13">
+      <c r="A36" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="B36" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C34" s="18"/>
-      <c r="D34" s="6"/>
-      <c r="E34" s="6"/>
-      <c r="F34" s="6"/>
-      <c r="G34" s="6"/>
-      <c r="H34" s="6"/>
-      <c r="I34" s="6"/>
-      <c r="J34" s="6"/>
-      <c r="K34" s="13"/>
-      <c r="L34" s="13"/>
-    </row>
-    <row r="35" spans="1:12">
-      <c r="A35" s="2"/>
-      <c r="B35" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="C35" s="18"/>
-      <c r="D35" s="6"/>
-      <c r="E35" s="6"/>
-      <c r="F35" s="6"/>
-      <c r="G35" s="6"/>
-      <c r="H35" s="6"/>
-      <c r="I35" s="6"/>
-      <c r="J35" s="6"/>
-      <c r="K35" s="13"/>
-      <c r="L35" s="13"/>
-    </row>
-    <row r="36" spans="1:12">
-      <c r="A36" s="2"/>
-      <c r="B36" s="2"/>
       <c r="C36" s="15"/>
-      <c r="D36" s="2"/>
-      <c r="E36" s="2"/>
-      <c r="F36" s="2"/>
-      <c r="G36" s="2"/>
-      <c r="H36" s="2"/>
-      <c r="I36" s="2"/>
-      <c r="J36" s="2"/>
-      <c r="K36" s="13"/>
-      <c r="L36" s="13"/>
-    </row>
-    <row r="37" spans="1:12">
-      <c r="A37" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="B37" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="C37" s="19"/>
-      <c r="D37" s="13"/>
-      <c r="E37" s="13"/>
-      <c r="F37" s="13"/>
-      <c r="G37" s="13"/>
-      <c r="H37" s="13"/>
-      <c r="I37" s="13"/>
-      <c r="J37" s="13"/>
-      <c r="K37" s="13"/>
-      <c r="L37" s="13"/>
+      <c r="D36" s="6"/>
+      <c r="E36" s="6"/>
+      <c r="F36" s="6"/>
+      <c r="G36" s="6"/>
+      <c r="H36" s="6"/>
+      <c r="I36" s="6"/>
+      <c r="J36" s="6"/>
+      <c r="K36" s="6"/>
+      <c r="L36" s="10"/>
+      <c r="M36" s="10"/>
+    </row>
+    <row r="37" spans="1:13">
+      <c r="A37" s="2"/>
+      <c r="B37" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C37" s="15"/>
+      <c r="D37" s="6"/>
+      <c r="E37" s="6"/>
+      <c r="F37" s="6"/>
+      <c r="G37" s="6"/>
+      <c r="H37" s="6"/>
+      <c r="I37" s="6"/>
+      <c r="J37" s="6"/>
+      <c r="K37" s="6"/>
+      <c r="L37" s="10"/>
+      <c r="M37" s="10"/>
+    </row>
+    <row r="38" spans="1:13">
+      <c r="A38" s="2"/>
+      <c r="B38" s="2"/>
+      <c r="C38" s="12"/>
+      <c r="D38" s="2"/>
+      <c r="E38" s="2"/>
+      <c r="F38" s="2"/>
+      <c r="G38" s="2"/>
+      <c r="H38" s="2"/>
+      <c r="I38" s="2"/>
+      <c r="J38" s="2"/>
+      <c r="K38" s="2"/>
+      <c r="L38" s="10"/>
+      <c r="M38" s="10"/>
+    </row>
+    <row r="39" spans="1:13">
+      <c r="A39" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="B39" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="C39" s="16"/>
+      <c r="D39" s="10"/>
+      <c r="E39" s="10"/>
+      <c r="F39" s="10"/>
+      <c r="G39" s="10"/>
+      <c r="H39" s="10"/>
+      <c r="I39" s="10"/>
+      <c r="J39" s="10"/>
+      <c r="K39" s="10"/>
+      <c r="L39" s="10"/>
+      <c r="M39" s="10"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="E22:H22"/>
-    <mergeCell ref="I22:J22"/>
-    <mergeCell ref="K22:L22"/>
+  <mergeCells count="6">
+    <mergeCell ref="J23:K23"/>
+    <mergeCell ref="L23:M23"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E23:I23"/>
+    <mergeCell ref="E32:F32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>